<commit_message>
changed file structure and accessibility ids
</commit_message>
<xml_diff>
--- a/target/classes/testData/ExcelFiles/Countries.xlsx
+++ b/target/classes/testData/ExcelFiles/Countries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awhitten/IdeaProjects/Iceberg/src/main/java/testData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bbakare/uitesting/src/main/java/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C838C6-E042-BF47-99CE-090EDB7F745A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0AEEBF-7E1A-4346-8F68-50BE35EEA284}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{FC1E2CE2-B3AF-F448-B6BA-BF974E11F672}"/>
+    <workbookView xWindow="440" yWindow="680" windowWidth="23180" windowHeight="18000" xr2:uid="{FC1E2CE2-B3AF-F448-B6BA-BF974E11F672}"/>
   </bookViews>
   <sheets>
     <sheet name="Countries" sheetId="1" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t>Armenia</t>
   </si>
   <si>
-    <t>Netherlands Antilles</t>
-  </si>
-  <si>
     <t>Angola</t>
   </si>
   <si>
@@ -81,9 +78,6 @@
     <t>Azerbaijan</t>
   </si>
   <si>
-    <t>Bosnia and Herzegovina</t>
-  </si>
-  <si>
     <t>Barbados</t>
   </si>
   <si>
@@ -108,9 +102,6 @@
     <t>Benin</t>
   </si>
   <si>
-    <t>Saint Barthélemy</t>
-  </si>
-  <si>
     <t>Bermuda</t>
   </si>
   <si>
@@ -300,9 +291,6 @@
     <t>Hong Kong [China]</t>
   </si>
   <si>
-    <t>Heard Island and McDonald Islands</t>
-  </si>
-  <si>
     <t>Honduras</t>
   </si>
   <si>
@@ -372,9 +360,6 @@
     <t>Comoros</t>
   </si>
   <si>
-    <t>Saint Kitts and Nevis</t>
-  </si>
-  <si>
     <t>North Korea</t>
   </si>
   <si>
@@ -396,9 +381,6 @@
     <t>Lebanon</t>
   </si>
   <si>
-    <t>Saint Lucia</t>
-  </si>
-  <si>
     <t>Liechtenstein</t>
   </si>
   <si>
@@ -435,9 +417,6 @@
     <t>Montenegro</t>
   </si>
   <si>
-    <t>Saint Martin</t>
-  </si>
-  <si>
     <t>Madagascar</t>
   </si>
   <si>
@@ -600,9 +579,6 @@
     <t>Singapore</t>
   </si>
   <si>
-    <t>Saint Helena</t>
-  </si>
-  <si>
     <t>Slovenia</t>
   </si>
   <si>
@@ -624,9 +600,6 @@
     <t>Suriname</t>
   </si>
   <si>
-    <t>São Tomé and Príncipe</t>
-  </si>
-  <si>
     <t>El Salvador</t>
   </si>
   <si>
@@ -636,9 +609,6 @@
     <t>Swaziland</t>
   </si>
   <si>
-    <t>Turks and Caicos Islands</t>
-  </si>
-  <si>
     <t>Chad</t>
   </si>
   <si>
@@ -672,9 +642,6 @@
     <t>Turkey</t>
   </si>
   <si>
-    <t>Trinidad and Tobago</t>
-  </si>
-  <si>
     <t>Tuvalu</t>
   </si>
   <si>
@@ -702,9 +669,6 @@
     <t>Vatican City</t>
   </si>
   <si>
-    <t>Saint Vincent and the Grenadines</t>
-  </si>
-  <si>
     <t>Venezuela</t>
   </si>
   <si>
@@ -720,9 +684,6 @@
     <t>Vanuatu</t>
   </si>
   <si>
-    <t>Wallis and Futuna</t>
-  </si>
-  <si>
     <t>Samoa</t>
   </si>
   <si>
@@ -751,6 +712,45 @@
   </si>
   <si>
     <t>Antigua &amp; Barbuda</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bosnia </t>
+  </si>
+  <si>
+    <t>St. Barthélemy</t>
+  </si>
+  <si>
+    <t>St. Helena</t>
+  </si>
+  <si>
+    <t>St. Kitts and Nevis</t>
+  </si>
+  <si>
+    <t>St. Lucia</t>
+  </si>
+  <si>
+    <t>St. Martin</t>
+  </si>
+  <si>
+    <t>Trinidad &amp; Tobago</t>
+  </si>
+  <si>
+    <t>São Tomé &amp; Príncipe</t>
+  </si>
+  <si>
+    <t>St. Vincent &amp; Grenadines</t>
+  </si>
+  <si>
+    <t>Turks &amp; Caicos Islands</t>
+  </si>
+  <si>
+    <t>Wallis &amp; Futuna</t>
+  </si>
+  <si>
+    <t>Heard &amp; McDonald Islands</t>
   </si>
 </sst>
 </file>
@@ -1121,8 +1121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDAE102C-5A99-5E49-A6E3-9E24F8DF11B6}">
   <dimension ref="A1:D242"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1139,49 +1139,49 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B3" s="2"/>
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>241</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2"/>
       <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B5" s="2"/>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2"/>
       <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2"/>
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B8" s="2"/>
       <c r="D8" s="3"/>
@@ -1195,42 +1195,42 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>10</v>
+        <v>228</v>
       </c>
       <c r="B10" s="2"/>
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2"/>
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B12" s="2"/>
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B13" s="2"/>
       <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="2"/>
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B15" s="2"/>
       <c r="D15" s="3"/>
@@ -1244,49 +1244,49 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B17" s="2"/>
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B18" s="2"/>
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="2"/>
       <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B20" s="2"/>
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B21" s="2"/>
       <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B22" s="2"/>
       <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B23" s="2"/>
       <c r="D23" s="3"/>
@@ -1307,7 +1307,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B26" s="2"/>
       <c r="D26" s="3"/>
@@ -1321,336 +1321,336 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>28</v>
+        <v>230</v>
       </c>
       <c r="B28" s="2"/>
       <c r="D28" s="3"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B29" s="2"/>
       <c r="D29" s="3"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B30" s="2"/>
       <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B31" s="2"/>
       <c r="D31" s="3"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="B32" s="2"/>
       <c r="D32" s="3"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>33</v>
+        <v>215</v>
       </c>
       <c r="B33" s="2"/>
       <c r="D33" s="3"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B34" s="2"/>
       <c r="D34" s="3"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="B35" s="2"/>
       <c r="D35" s="3"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B36" s="2"/>
       <c r="D36" s="3"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B37" s="2"/>
       <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>38</v>
+        <v>108</v>
       </c>
       <c r="B38" s="2"/>
       <c r="D38" s="3"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B39" s="2"/>
       <c r="D39" s="3"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B40" s="2"/>
       <c r="D40" s="3"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B41" s="2"/>
       <c r="D41" s="3"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>42</v>
+        <v>114</v>
       </c>
       <c r="B42" s="2"/>
       <c r="D42" s="3"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B43" s="2"/>
       <c r="D43" s="3"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>44</v>
+        <v>194</v>
       </c>
       <c r="B44" s="2"/>
       <c r="D44" s="3"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B45" s="2"/>
       <c r="D45" s="3"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B46" s="2"/>
       <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B47" s="2"/>
       <c r="D47" s="3"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="B48" s="2"/>
       <c r="D48" s="3"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B49" s="2"/>
       <c r="D49" s="3"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="B50" s="2"/>
       <c r="D50" s="3"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B51" s="2"/>
       <c r="D51" s="3"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="B52" s="2"/>
       <c r="D52" s="3"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B53" s="2"/>
       <c r="D53" s="3"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B54" s="2"/>
       <c r="D54" s="3"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>240</v>
+        <v>41</v>
       </c>
       <c r="B55" s="2"/>
       <c r="D55" s="3"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="B56" s="2"/>
       <c r="D56" s="3"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B57" s="2"/>
       <c r="D57" s="3"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B58" s="2"/>
       <c r="D58" s="3"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>58</v>
+        <v>227</v>
       </c>
       <c r="B59" s="2"/>
       <c r="D59" s="3"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B60" s="2"/>
       <c r="D60" s="3"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="B61" s="2"/>
       <c r="D61" s="3"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="B62" s="2"/>
       <c r="D62" s="3"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B63" s="2"/>
       <c r="D63" s="3"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>61</v>
+        <v>3</v>
       </c>
       <c r="B64" s="2"/>
       <c r="D64" s="3"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B65" s="2"/>
       <c r="D65" s="3"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>63</v>
+        <v>191</v>
       </c>
       <c r="B66" s="2"/>
       <c r="D66" s="3"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="B67" s="2"/>
       <c r="D67" s="3"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B68" s="2"/>
       <c r="D68" s="3"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B69" s="2"/>
       <c r="D69" s="3"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B70" s="2"/>
       <c r="D70" s="3"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B71" s="2"/>
       <c r="D71" s="3"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B72" s="2"/>
       <c r="D72" s="3"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B73" s="2"/>
       <c r="D73" s="3"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B74" s="2"/>
       <c r="D74" s="3"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B75" s="2"/>
       <c r="D75" s="3"/>
@@ -1664,56 +1664,56 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>74</v>
+        <v>161</v>
       </c>
       <c r="B77" s="2"/>
       <c r="D77" s="3"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>75</v>
+        <v>195</v>
       </c>
       <c r="B78" s="2"/>
       <c r="D78" s="3"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B79" s="2"/>
       <c r="D79" s="3"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B80" s="2"/>
       <c r="D80" s="3"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B81" s="2"/>
       <c r="D81" s="3"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="B82" s="2"/>
       <c r="D82" s="3"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B83" s="2"/>
       <c r="D83" s="3"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B84" s="2"/>
       <c r="D84" s="3"/>
@@ -1727,119 +1727,119 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B86" s="2"/>
       <c r="D86" s="3"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B87" s="2"/>
       <c r="D87" s="3"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B88" s="2"/>
       <c r="D88" s="3"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>239</v>
+        <v>84</v>
       </c>
       <c r="B89" s="2"/>
       <c r="D89" s="3"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B90" s="2"/>
       <c r="D90" s="3"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="B91" s="2"/>
       <c r="D91" s="3"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B92" s="2"/>
       <c r="D92" s="3"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B93" s="2"/>
       <c r="D93" s="3"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B94" s="2"/>
       <c r="D94" s="3"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B95" s="2"/>
       <c r="D95" s="3"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>92</v>
+        <v>241</v>
       </c>
       <c r="B96" s="2"/>
       <c r="D96" s="3"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B97" s="2"/>
       <c r="D97" s="3"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B98" s="2"/>
       <c r="D98" s="3"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B99" s="2"/>
       <c r="D99" s="3"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B100" s="2"/>
       <c r="D100" s="3"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B101" s="2"/>
       <c r="D101" s="3"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B102" s="2"/>
       <c r="D102" s="3"/>
@@ -1853,217 +1853,217 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B104" s="2"/>
       <c r="D104" s="3"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B105" s="2"/>
       <c r="D105" s="3"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B106" s="2"/>
       <c r="D106" s="3"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B107" s="2"/>
       <c r="D107" s="3"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B108" s="2"/>
       <c r="D108" s="3"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B109" s="2"/>
       <c r="D109" s="3"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B110" s="2"/>
       <c r="D110" s="3"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B111" s="2"/>
       <c r="D111" s="3"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B112" s="2"/>
       <c r="D112" s="3"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B113" s="2"/>
       <c r="D113" s="3"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B114" s="2"/>
       <c r="D114" s="3"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B115" s="2"/>
       <c r="D115" s="3"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B116" s="2"/>
       <c r="D116" s="3"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B117" s="2"/>
       <c r="D117" s="3"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B118" s="2"/>
       <c r="D118" s="3"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="B119" s="2"/>
       <c r="D119" s="3"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B120" s="2"/>
       <c r="D120" s="3"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B121" s="2"/>
       <c r="D121" s="3"/>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B122" s="2"/>
       <c r="D122" s="3"/>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B123" s="2"/>
       <c r="D123" s="3"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B124" s="2"/>
       <c r="D124" s="3"/>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B125" s="2"/>
       <c r="D125" s="3"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B126" s="2"/>
       <c r="D126" s="3"/>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
-        <v>123</v>
+        <v>225</v>
       </c>
       <c r="B127" s="2"/>
       <c r="D127" s="3"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="B128" s="2"/>
       <c r="D128" s="3"/>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B129" s="2"/>
       <c r="D129" s="3"/>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="B130" s="2"/>
       <c r="D130" s="3"/>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
-        <v>127</v>
+        <v>145</v>
       </c>
       <c r="B131" s="2"/>
       <c r="D131" s="3"/>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="B132" s="2"/>
       <c r="D132" s="3"/>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B133" s="2"/>
       <c r="D133" s="3"/>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="B134" s="2"/>
       <c r="D134" s="3"/>
@@ -2077,287 +2077,287 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="B136" s="2"/>
       <c r="D136" s="3"/>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="B137" s="2"/>
       <c r="D137" s="3"/>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="B138" s="2"/>
       <c r="D138" s="3"/>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
-        <v>135</v>
+        <v>221</v>
       </c>
       <c r="B139" s="2"/>
       <c r="D139" s="3"/>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="B140" s="2"/>
       <c r="D140" s="3"/>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
-        <v>137</v>
+        <v>66</v>
       </c>
       <c r="B141" s="2"/>
       <c r="D141" s="3"/>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="B142" s="2"/>
       <c r="D142" s="3"/>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="B143" s="2"/>
       <c r="D143" s="3"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
-        <v>238</v>
+        <v>135</v>
       </c>
       <c r="B144" s="2"/>
       <c r="D144" s="3"/>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="B145" s="2"/>
       <c r="D145" s="3"/>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B146" s="2"/>
       <c r="D146" s="3"/>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="B147" s="2"/>
       <c r="D147" s="3"/>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B148" s="2"/>
       <c r="D148" s="3"/>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="B149" s="2"/>
       <c r="D149" s="3"/>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B150" s="2"/>
       <c r="D150" s="3"/>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="B151" s="2"/>
       <c r="D151" s="3"/>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B152" s="2"/>
       <c r="D152" s="3"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
-        <v>148</v>
+        <v>229</v>
       </c>
       <c r="B153" s="2"/>
       <c r="D153" s="3"/>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B154" s="2"/>
       <c r="D154" s="3"/>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="B155" s="2"/>
       <c r="D155" s="3"/>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B156" s="2"/>
       <c r="D156" s="3"/>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B157" s="2"/>
       <c r="D157" s="3"/>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B158" s="2"/>
       <c r="D158" s="3"/>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B159" s="2"/>
       <c r="D159" s="3"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B160" s="2"/>
       <c r="D160" s="3"/>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
-        <v>156</v>
+        <v>111</v>
       </c>
       <c r="B161" s="2"/>
       <c r="D161" s="3"/>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="B162" s="2"/>
       <c r="D162" s="3"/>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B163" s="2"/>
       <c r="D163" s="3"/>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B164" s="2"/>
       <c r="D164" s="3"/>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B165" s="2"/>
       <c r="D165" s="3"/>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="B166" s="2"/>
       <c r="D166" s="3"/>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="B167" s="2"/>
       <c r="D167" s="3"/>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B168" s="2"/>
       <c r="D168" s="3"/>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B169" s="2"/>
       <c r="D169" s="3"/>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="B170" s="2"/>
       <c r="D170" s="3"/>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B171" s="2"/>
       <c r="D171" s="3"/>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B172" s="2"/>
       <c r="D172" s="3"/>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B173" s="2"/>
       <c r="D173" s="3"/>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B174" s="2"/>
       <c r="D174" s="3"/>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B175" s="2"/>
       <c r="D175" s="3"/>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B176" s="2"/>
       <c r="D176" s="3"/>
@@ -2385,446 +2385,449 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B180" s="2"/>
       <c r="D180" s="3"/>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B181" s="2"/>
       <c r="D181" s="3"/>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" s="2" t="s">
-        <v>177</v>
+        <v>219</v>
       </c>
       <c r="B182" s="2"/>
       <c r="D182" s="3"/>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" s="2" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="B183" s="2"/>
       <c r="D183" s="3"/>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" s="2" t="s">
-        <v>179</v>
+        <v>237</v>
       </c>
       <c r="B184" s="2"/>
       <c r="D184" s="3"/>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B185" s="2"/>
       <c r="D185" s="3"/>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" s="2" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="B186" s="2"/>
       <c r="D186" s="3"/>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" s="2" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B187" s="2"/>
       <c r="D187" s="3"/>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B188" s="2"/>
       <c r="D188" s="3"/>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" s="2" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B189" s="2"/>
       <c r="D189" s="3"/>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B190" s="2"/>
       <c r="D190" s="3"/>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B191" s="2"/>
       <c r="D191" s="3"/>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B192" s="2"/>
       <c r="D192" s="3"/>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" s="2" t="s">
-        <v>188</v>
+        <v>226</v>
       </c>
       <c r="B193" s="2"/>
       <c r="D193" s="3"/>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" s="2" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="B194" s="2"/>
       <c r="D194" s="3"/>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B195" s="2"/>
       <c r="D195" s="3"/>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" s="2" t="s">
-        <v>191</v>
+        <v>222</v>
       </c>
       <c r="B196" s="2"/>
       <c r="D196" s="3"/>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197" s="2" t="s">
-        <v>192</v>
+        <v>112</v>
       </c>
       <c r="B197" s="2"/>
       <c r="D197" s="3"/>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" s="2" t="s">
-        <v>193</v>
+        <v>61</v>
       </c>
       <c r="B198" s="2"/>
       <c r="D198" s="3"/>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" s="2" t="s">
-        <v>194</v>
+        <v>119</v>
       </c>
       <c r="B199" s="2"/>
       <c r="D199" s="3"/>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" s="2" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
       <c r="B200" s="2"/>
       <c r="D200" s="3"/>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201" s="2" t="s">
-        <v>196</v>
+        <v>232</v>
       </c>
       <c r="B201" s="2"/>
       <c r="D201" s="3"/>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202" s="2" t="s">
-        <v>197</v>
+        <v>233</v>
       </c>
       <c r="B202" s="2"/>
       <c r="D202" s="3"/>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A203" s="2" t="s">
-        <v>198</v>
+        <v>234</v>
       </c>
       <c r="B203" s="2"/>
       <c r="D203" s="3"/>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204" s="2" t="s">
-        <v>199</v>
+        <v>235</v>
       </c>
       <c r="B204" s="2"/>
       <c r="D204" s="3"/>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" s="2" t="s">
-        <v>200</v>
+        <v>238</v>
       </c>
       <c r="B205" s="2"/>
       <c r="D205" s="3"/>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206" s="2" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="B206" s="2"/>
       <c r="D206" s="3"/>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207" s="2" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="B207" s="2"/>
       <c r="D207" s="3"/>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A208" s="2" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="B208" s="2"/>
       <c r="D208" s="3"/>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A209" s="2" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="B209" s="2"/>
       <c r="D209" s="3"/>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A210" s="2" t="s">
-        <v>205</v>
+        <v>40</v>
       </c>
       <c r="B210" s="2"/>
       <c r="D210" s="3"/>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A211" s="2" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="B211" s="2"/>
       <c r="D211" s="3"/>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A212" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B212" s="2"/>
       <c r="D212" s="3"/>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A213" s="2" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B213" s="2"/>
       <c r="D213" s="3"/>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A214" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B214" s="2"/>
       <c r="D214" s="3"/>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A215" s="2" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="B215" s="2"/>
       <c r="D215" s="3"/>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A216" s="2" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="B216" s="2"/>
       <c r="D216" s="3"/>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A217" s="2" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="B217" s="2"/>
       <c r="D217" s="3"/>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A218" s="2" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="B218" s="2"/>
       <c r="D218" s="3"/>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A219" s="2" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="B219" s="2"/>
       <c r="D219" s="3"/>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A220" s="2" t="s">
-        <v>215</v>
+        <v>236</v>
       </c>
       <c r="B220" s="2"/>
       <c r="D220" s="3"/>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A221" s="2" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="B221" s="2"/>
       <c r="D221" s="3"/>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A222" s="2" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="B222" s="2"/>
       <c r="D222" s="3"/>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A223" s="2" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="B223" s="2"/>
       <c r="D223" s="3"/>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A224" s="2" t="s">
-        <v>219</v>
+        <v>239</v>
       </c>
       <c r="B224" s="2"/>
       <c r="D224" s="3"/>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A225" s="2" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="B225" s="2"/>
       <c r="D225" s="3"/>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A226" s="2" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B226" s="2"/>
       <c r="D226" s="3"/>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A227" s="2" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="B227" s="2"/>
       <c r="D227" s="3"/>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A228" s="2" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="B228" s="2"/>
       <c r="D228" s="3"/>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A229" s="2" t="s">
-        <v>224</v>
+        <v>1</v>
       </c>
       <c r="B229" s="2"/>
       <c r="D229" s="3"/>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A230" s="2" t="s">
-        <v>225</v>
+        <v>70</v>
       </c>
       <c r="B230" s="2"/>
       <c r="D230" s="3"/>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A231" s="2" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="B231" s="2"/>
       <c r="D231" s="3"/>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A232" s="2" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="B232" s="2"/>
       <c r="D232" s="3"/>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A233" s="2" t="s">
-        <v>228</v>
+        <v>212</v>
       </c>
       <c r="B233" s="2"/>
       <c r="D233" s="3"/>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A234" s="2" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="B234" s="2"/>
       <c r="D234" s="3"/>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A235" s="2" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
       <c r="B235" s="2"/>
       <c r="D235" s="3"/>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A236" s="2" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
       <c r="B236" s="2"/>
       <c r="D236" s="3"/>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A237" s="2" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="B237" s="2"/>
       <c r="D237" s="3"/>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A238" s="2" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="B238" s="2"/>
       <c r="D238" s="3"/>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A239" s="2" t="s">
-        <v>234</v>
+        <v>59</v>
       </c>
       <c r="B239" s="2"/>
       <c r="D239" s="3"/>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A240" s="2" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="B240" s="2"/>
       <c r="D240" s="3"/>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A241" s="2" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="B241" s="2"/>
       <c r="D241" s="3"/>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A242" s="2" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="B242" s="2"/>
       <c r="D242" s="3"/>
     </row>
   </sheetData>
+  <sortState ref="A2:A242">
+    <sortCondition ref="A190"/>
+  </sortState>
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>